<commit_message>
add main payment report
</commit_message>
<xml_diff>
--- a/app/erp/module/prop_report_rent_payment/excel/prop_report_rent_payment_template_v01.xlsx
+++ b/app/erp/module/prop_report_rent_payment/excel/prop_report_rent_payment_template_v01.xlsx
@@ -55,9 +55,6 @@
     <t>Invoice No.</t>
   </si>
   <si>
-    <t>Report: Rent Payment Report</t>
-  </si>
-  <si>
     <t>Payment Date</t>
   </si>
   <si>
@@ -74,6 +71,9 @@
   </si>
   <si>
     <t>Period Date To</t>
+  </si>
+  <si>
+    <t>Report: Rent Payment Report</t>
   </si>
 </sst>
 </file>
@@ -1058,7 +1058,9 @@
   </sheetPr>
   <dimension ref="A1:N2801"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1076,7 +1078,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="8"/>
@@ -1154,10 +1156,10 @@
         <v>5</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>6</v>
@@ -1178,16 +1180,16 @@
         <v>11</v>
       </c>
       <c r="K5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="7" t="s">
-        <v>18</v>
-      </c>
       <c r="M5" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N5" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>